<commit_message>
Correctie foutje bij normalisatie dierenkliniek
</commit_message>
<xml_diff>
--- a/resources/dierenkliniek.xlsx
+++ b/resources/dierenkliniek.xlsx
@@ -1,15 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="18625"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="29328"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\benw\Documenten\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\studieboeken\leeraccess\resources\"/>
     </mc:Choice>
   </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D2BA0C68-8C4E-4F6C-8A4D-001DFE6F3ECF}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="13650" windowHeight="7155" xr2:uid="{BCB87582-9A87-4DDC-AD78-8CFA87B3BFB0}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="30936" windowHeight="16776" xr2:uid="{BCB87582-9A87-4DDC-AD78-8CFA87B3BFB0}"/>
   </bookViews>
   <sheets>
     <sheet name="animal_clinic" sheetId="1" r:id="rId1"/>
@@ -80,9 +81,6 @@
     <t>04 - Tetanus vaccinatie</t>
   </si>
   <si>
-    <t xml:space="preserve">11 - Oogonsteking </t>
-  </si>
-  <si>
     <t>21 - Jaarlijkse controle</t>
   </si>
   <si>
@@ -93,6 +91,9 @@
   </si>
   <si>
     <t>10 - Wondbehandeling</t>
+  </si>
+  <si>
+    <t xml:space="preserve">11 - Oogontsteking </t>
   </si>
 </sst>
 </file>
@@ -102,7 +103,7 @@
   <numFmts count="1">
     <numFmt numFmtId="164" formatCode="dd/mm/yyyy"/>
   </numFmts>
-  <fonts count="3" x14ac:knownFonts="1">
+  <fonts count="2" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -112,14 +113,7 @@
     </font>
     <font>
       <b/>
-      <sz val="10"/>
-      <color theme="1"/>
-      <name val="Calibri"/>
-      <family val="2"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="10"/>
+      <sz val="11"/>
       <color theme="1"/>
       <name val="Calibri"/>
       <family val="2"/>
@@ -149,14 +143,14 @@
   <cellXfs count="6">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="164" fontId="2" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Standaard" xfId="0" builtinId="0"/>
@@ -175,9 +169,9 @@
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Kantoorthema">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office 2013 - 2022 Thema">
   <a:themeElements>
-    <a:clrScheme name="Office">
+    <a:clrScheme name="Office 2013 - 2022">
       <a:dk1>
         <a:sysClr val="windowText" lastClr="000000"/>
       </a:dk1>
@@ -215,7 +209,7 @@
         <a:srgbClr val="954F72"/>
       </a:folHlink>
     </a:clrScheme>
-    <a:fontScheme name="Office">
+    <a:fontScheme name="Office 2013 - 2022">
       <a:majorFont>
         <a:latin typeface="Calibri Light" panose="020F0302020204030204"/>
         <a:ea typeface=""/>
@@ -321,7 +315,7 @@
         <a:font script="Tfng" typeface="Ebrima"/>
       </a:minorFont>
     </a:fontScheme>
-    <a:fmtScheme name="Office">
+    <a:fmtScheme name="Office 2013 - 2022">
       <a:fillStyleLst>
         <a:solidFill>
           <a:schemeClr val="phClr"/>
@@ -463,7 +457,7 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office 2013 - 2022 Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
@@ -474,22 +468,22 @@
   <dimension ref="A1:G14"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="T14" sqref="T14"/>
+      <selection activeCell="I19" sqref="I19"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultColWidth="9.109375" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="5.85546875" style="2" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="8.42578125" style="2" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="7.7109375" style="2" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="6.5703125" style="2" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="13.28515625" style="2" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="11.7109375" style="2" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="19.42578125" style="2" bestFit="1" customWidth="1"/>
-    <col min="8" max="16384" width="9.140625" style="2"/>
+    <col min="1" max="1" width="6" style="2" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="9" style="2" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="8" style="2" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="6.88671875" style="2" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="13.77734375" style="2" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="12.5546875" style="2" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="19.88671875" style="2" bestFit="1" customWidth="1"/>
+    <col min="8" max="16384" width="9.109375" style="2"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A1" s="1" t="s">
         <v>1</v>
       </c>
@@ -512,7 +506,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="2" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A2" s="3">
         <v>123</v>
       </c>
@@ -535,37 +529,37 @@
         <v>16</v>
       </c>
     </row>
-    <row r="3" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A3" s="3"/>
       <c r="D3" s="3"/>
       <c r="F3" s="5">
         <v>42454</v>
       </c>
       <c r="G3" s="2" t="s">
-        <v>22</v>
-      </c>
-    </row>
-    <row r="4" spans="1:7" x14ac:dyDescent="0.2">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="4" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A4" s="3"/>
       <c r="D4" s="3"/>
       <c r="F4" s="5">
         <v>42466</v>
       </c>
       <c r="G4" s="2" t="s">
-        <v>20</v>
-      </c>
-    </row>
-    <row r="5" spans="1:7" x14ac:dyDescent="0.2">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="5" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A5" s="3"/>
       <c r="D5" s="3"/>
       <c r="F5" s="5"/>
     </row>
-    <row r="6" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A6" s="3"/>
       <c r="D6" s="3"/>
       <c r="F6" s="5"/>
     </row>
-    <row r="7" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A7" s="3">
         <v>149</v>
       </c>
@@ -588,22 +582,22 @@
         <v>17</v>
       </c>
     </row>
-    <row r="8" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="8" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A8" s="3"/>
       <c r="D8" s="3"/>
       <c r="F8" s="5">
         <v>42444</v>
       </c>
       <c r="G8" s="2" t="s">
-        <v>21</v>
-      </c>
-    </row>
-    <row r="9" spans="1:7" x14ac:dyDescent="0.2">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="9" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A9" s="3"/>
       <c r="D9" s="3"/>
       <c r="F9" s="5"/>
     </row>
-    <row r="10" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="10" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A10" s="3">
         <v>170</v>
       </c>
@@ -626,7 +620,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="11" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="11" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A11" s="3"/>
       <c r="D11" s="3"/>
       <c r="F11" s="5">
@@ -636,12 +630,12 @@
         <v>16</v>
       </c>
     </row>
-    <row r="12" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="12" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A12" s="3"/>
       <c r="D12" s="3"/>
       <c r="F12" s="5"/>
     </row>
-    <row r="13" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="13" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A13" s="3">
         <v>260</v>
       </c>
@@ -661,15 +655,15 @@
         <v>42487</v>
       </c>
       <c r="G13" s="2" t="s">
-        <v>19</v>
-      </c>
-    </row>
-    <row r="14" spans="1:7" x14ac:dyDescent="0.2">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="14" spans="1:7" x14ac:dyDescent="0.3">
       <c r="F14" s="5">
         <v>42487</v>
       </c>
       <c r="G14" s="2" t="s">
-        <v>18</v>
+        <v>22</v>
       </c>
     </row>
   </sheetData>

</xml_diff>